<commit_message>
Mise à jour du glossaire
</commit_message>
<xml_diff>
--- a/glossaire.xlsx
+++ b/glossaire.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\02Pro Tom Press\heuresSupTPV3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8678625-3D2D-4606-A33D-652ADD168E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5FE85F-9FB0-49A2-9381-8E73EEC53732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28935" yWindow="-2070" windowWidth="29070" windowHeight="18270" tabRatio="476" activeTab="1" xr2:uid="{2D9FC5F1-BAE4-4CE5-BAE7-1CF8E3ADBA7C}"/>
+    <workbookView xWindow="-28920" yWindow="-2055" windowWidth="29040" windowHeight="18240" tabRatio="476" activeTab="1" xr2:uid="{2D9FC5F1-BAE4-4CE5-BAE7-1CF8E3ADBA7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil2!$A$1:$F$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil2!$A$1:$G$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="189">
   <si>
     <t>//Fonction isvalid contrôle la cohérence matricule/mot de passe</t>
   </si>
@@ -520,6 +520,93 @@
   </si>
   <si>
     <t>Valide la semaine du responsable connecté</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vient de </t>
+  </si>
+  <si>
+    <t>envoie vers</t>
+  </si>
+  <si>
+    <t>accueil</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>validationresp;accueil</t>
+  </si>
+  <si>
+    <t>index et tout autres pages si pas connecté</t>
+  </si>
+  <si>
+    <t>adminApayer</t>
+  </si>
+  <si>
+    <t>accueil;index</t>
+  </si>
+  <si>
+    <t>index;actionPayeHeure</t>
+  </si>
+  <si>
+    <t>index;accueil</t>
+  </si>
+  <si>
+    <t>adminDetailheures</t>
+  </si>
+  <si>
+    <t>enregistre</t>
+  </si>
+  <si>
+    <t>ouverture</t>
+  </si>
+  <si>
+    <t>okmdp</t>
+  </si>
+  <si>
+    <t>index;okmdp</t>
+  </si>
+  <si>
+    <t>index;userAdd</t>
+  </si>
+  <si>
+    <t>index;userList;actionMDPTemporaire</t>
+  </si>
+  <si>
+    <t>index;userEdit</t>
+  </si>
+  <si>
+    <t>index;actionOKHeure;actionAnnulerHeure</t>
+  </si>
+  <si>
+    <t>actions/logout</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
+    <t>index;function petitsVieux()</t>
+  </si>
+  <si>
+    <t>actionAnnulerHeure;actionOKHeure;actionOKPayerHeure;navbar</t>
+  </si>
+  <si>
+    <t>adminptitvieux;navbar</t>
+  </si>
+  <si>
+    <t>actionPayeHeure;navbar</t>
+  </si>
+  <si>
+    <t>userList;navbar</t>
+  </si>
+  <si>
+    <t>userEdit;navbar</t>
+  </si>
+  <si>
+    <t>permanent</t>
   </si>
 </sst>
 </file>
@@ -541,7 +628,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,6 +638,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,12 +660,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -887,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B9AF25-689A-44CF-86A6-ED2E637BF27A}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,10 +995,10 @@
     <col min="2" max="2" width="51.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="99.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="76.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -921,8 +1017,11 @@
       <c r="F1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -942,7 +1041,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -962,7 +1061,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -982,7 +1081,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1002,7 +1101,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1022,7 +1121,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1042,7 +1141,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1062,7 +1161,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1082,7 +1181,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1102,7 +1201,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1122,7 +1221,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1142,7 +1241,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1162,7 +1261,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1182,7 +1281,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1202,7 +1301,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1222,7 +1321,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
@@ -1240,7 +1339,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
@@ -1258,7 +1357,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1278,7 +1377,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -1297,8 +1396,11 @@
       <c r="F20" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
@@ -1316,7 +1418,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1336,7 +1438,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1356,7 +1458,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1376,7 +1478,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1396,7 +1498,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -1413,7 +1515,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -1430,7 +1532,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -1447,7 +1549,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -1464,7 +1566,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -1481,7 +1583,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -1498,7 +1600,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -1899,7 +2001,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F54" xr:uid="{07B9AF25-689A-44CF-86A6-ED2E637BF27A}"/>
+  <autoFilter ref="A1:G54" xr:uid="{07B9AF25-689A-44CF-86A6-ED2E637BF27A}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="120" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1908,14 +2010,455 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68812287-F342-4FB6-9A5D-9E81F0310AB2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="H5" sqref="H5:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" t="s">
+        <v>169</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>188</v>
+      </c>
+      <c r="C27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>188</v>
+      </c>
+      <c r="C28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>188</v>
+      </c>
+      <c r="C30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>188</v>
+      </c>
+      <c r="C31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>188</v>
+      </c>
+      <c r="C33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" t="s">
+        <v>188</v>
+      </c>
+      <c r="C36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
+        <v>188</v>
+      </c>
+      <c r="C38" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>181</v>
+      </c>
+      <c r="B41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="120" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correction des solde initiaux à payer
</commit_message>
<xml_diff>
--- a/glossaire.xlsx
+++ b/glossaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\02Pro Tom Press\heuresSupTPV3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5FE85F-9FB0-49A2-9381-8E73EEC53732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD77D709-E797-4783-B045-1E8718954722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2055" windowWidth="29040" windowHeight="18240" tabRatio="476" activeTab="1" xr2:uid="{2D9FC5F1-BAE4-4CE5-BAE7-1CF8E3ADBA7C}"/>
   </bookViews>
@@ -2013,7 +2013,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:J13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ajout de l'historique sur l'accueil
</commit_message>
<xml_diff>
--- a/glossaire.xlsx
+++ b/glossaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\02Pro Tom Press\heuresSupTPV3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92B038D-FE77-402E-A4BD-018F6B6C474C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262E0931-B299-4DFD-A030-3662F5C32E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="476" xr2:uid="{2D9FC5F1-BAE4-4CE5-BAE7-1CF8E3ADBA7C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="197">
   <si>
     <t>//Fonction isvalid contrôle la cohérence matricule/mot de passe</t>
   </si>
@@ -625,6 +625,12 @@
   </si>
   <si>
     <t>Supprime l'heure sélectionnée</t>
+  </si>
+  <si>
+    <t>historiqueSemaineEnCours($Matricule,$pdo)</t>
+  </si>
+  <si>
+    <t>Donne l'historique des heures</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B9AF25-689A-44CF-86A6-ED2E637BF27A}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="B44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2050,6 +2056,23 @@
       </c>
       <c r="F56" t="s">
         <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" t="s">
+        <v>195</v>
+      </c>
+      <c r="C57" t="s">
+        <v>196</v>
+      </c>
+      <c r="D57" t="s">
+        <v>60</v>
+      </c>
+      <c r="F57" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>